<commit_message>
fix some bugs in userservice
</commit_message>
<xml_diff>
--- a/importproducts.xlsx
+++ b/importproducts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\project\product-manager-for-arius\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743D4D98-625A-4488-8684-157CAAFB4309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7509BA9-5AD0-49E5-818F-F562A0299C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39EFEBBD-D3D2-4888-A979-D32A270A3575}"/>
   </bookViews>
@@ -35,60 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="4">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="3"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="4">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-    <bk>
-      <rc t="1" v="1"/>
-    </bk>
-    <bk>
-      <rc t="1" v="2"/>
-    </bk>
-    <bk>
-      <rc t="1" v="3"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -136,13 +84,25 @@
   </si>
   <si>
     <t>nhanh, nhỏ gọn và nhẹ</t>
+  </si>
+  <si>
+    <t>https://kidskids.s3.us-east-2.amazonaws.com/quangduy/images/ip15promax1.jpg</t>
+  </si>
+  <si>
+    <t>https://kidskids.s3.us-east-2.amazonaws.com/quangduy/images/ip15promax.jpg</t>
+  </si>
+  <si>
+    <t>https://kidskids.s3.us-east-2.amazonaws.com/quangduy/images/laptop1.png</t>
+  </si>
+  <si>
+    <t>https://kidskids.s3.us-east-2.amazonaws.com/quangduy/images/laptop2.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +114,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,14 +144,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -197,85 +168,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>2</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>3</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-  <rel r:id="rId3"/>
-  <rel r:id="rId4"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,7 +490,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,11 +538,11 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C2" t="e" vm="2">
-        <v>#VALUE!</v>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D2">
         <v>20000000</v>
@@ -675,11 +567,11 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C3" t="e" vm="4">
-        <v>#VALUE!</v>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D3">
         <v>200000000</v>
@@ -701,7 +593,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7EDD98B3-2381-417A-87ED-BCD2B833DA62}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{F367B40A-94A5-4481-8B9E-B33158059CAB}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{54830694-7A06-4314-A3E9-9DE8DEF8D188}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{3206A75E-399F-4A18-81FA-0070AC5FDAD9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>